<commit_message>
Login related testcases without validation
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/credentials.xlsx
+++ b/src/test/resources/testdata/credentials.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaya/Documents/Selenium/sauseDemo/src/test/resources/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F33B7E65-CC8F-FB42-9468-2F8544E388AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1EF62BC-A64E-234D-8123-38A29022FCE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17120" xr2:uid="{83650D97-E557-484B-9A52-119491A8770E}"/>
   </bookViews>
   <sheets>
-    <sheet name="loginTest" sheetId="1" r:id="rId1"/>
+    <sheet name="loginTest" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,9 +37,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>userName</t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
@@ -47,6 +44,9 @@
   </si>
   <si>
     <t>secret_sauce</t>
+  </si>
+  <si>
+    <t>username</t>
   </si>
 </sst>
 </file>
@@ -397,33 +397,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A6484A4-C64F-DD42-B7D9-6E5CA1F26196}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AEF262E-9B95-164D-9010-4EE451456767}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.83203125" customWidth="1"/>
-    <col min="2" max="2" width="20.83203125" customWidth="1"/>
+    <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>